<commit_message>
Update additional figures and tables
</commit_message>
<xml_diff>
--- a/02_additional_figs_tables/STable_5.xlsx
+++ b/02_additional_figs_tables/STable_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Sync\00_Collabs\Ed_LUCA_v2\01_PAML\figs_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\Sync\00_Collabs\LUCA-divtimes\LUCA-divtimes\02_additional_figs_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C40EFD-6BF7-4E53-9908-B6DF880CE511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B482721-BDA4-4E93-B030-D7ECBD3E5D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="6" xr2:uid="{EA54679C-0783-464A-ACDF-78BEF02C3352}"/>
   </bookViews>
@@ -1043,37 +1043,19 @@
     <t>97.5%q-conc_cb</t>
   </si>
   <si>
-    <t>2.75%q-conc_notcb</t>
-  </si>
-  <si>
     <t>97.5%q-conc_notcb</t>
-  </si>
-  <si>
-    <t>2.75%q-conc_fosscb</t>
   </si>
   <si>
     <t>97.5%q-conc_fosscb</t>
   </si>
   <si>
-    <t>2.75%q-part_cb</t>
-  </si>
-  <si>
     <t>97.5%q-part_cb</t>
-  </si>
-  <si>
-    <t>2.75%q-part_notcb</t>
   </si>
   <si>
     <t>97.5%q-part_notcb</t>
   </si>
   <si>
-    <t>2.75%q-part_fosscb</t>
-  </si>
-  <si>
     <t>97.5%q-part_fosscb</t>
-  </si>
-  <si>
-    <t>2.75%q-conc_cb</t>
   </si>
   <si>
     <t>Num. samples used to calculate stats</t>
@@ -1086,6 +1068,24 @@
   </si>
   <si>
     <t>bulk-ESS (max. value across all chains)</t>
+  </si>
+  <si>
+    <t>2.5%q-conc_cb</t>
+  </si>
+  <si>
+    <t>2.5%q-conc_notcb</t>
+  </si>
+  <si>
+    <t>2.5%q-conc_fosscb</t>
+  </si>
+  <si>
+    <t>2.5%q-part_cb</t>
+  </si>
+  <si>
+    <t>2.5%q-part_notcb</t>
+  </si>
+  <si>
+    <t>2.5%q-part_fosscb</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31879A1C-71B8-4853-8146-BC6667CC099E}">
   <dimension ref="A1:S247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1468,7 +1468,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>69</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>332</v>
@@ -1516,46 +1516,46 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" t="s">
         <v>333</v>
-      </c>
-      <c r="G2" t="s">
-        <v>334</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="M2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="P2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="Q2" t="s">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -16031,8 +16031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF01B5CF-C1C0-4CAD-94FC-76B54AB414C9}">
   <dimension ref="A1:S247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16054,7 +16054,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>69</v>
@@ -16093,7 +16093,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>332</v>
@@ -16102,46 +16102,46 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" t="s">
         <v>333</v>
-      </c>
-      <c r="G2" t="s">
-        <v>334</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="M2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="P2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="Q2" t="s">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -30617,8 +30617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3413B57-BF9F-4A06-99D8-535412D9EFF9}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30640,7 +30640,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>69</v>
@@ -30679,7 +30679,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>332</v>
@@ -30688,46 +30688,46 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" t="s">
         <v>333</v>
-      </c>
-      <c r="G2" t="s">
-        <v>334</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="M2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="P2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="Q2" t="s">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -34465,8 +34465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4C1ED1-0EA7-4C1A-8577-F633A6651066}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34488,7 +34488,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>69</v>
@@ -34527,7 +34527,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>332</v>
@@ -34536,46 +34536,46 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" t="s">
         <v>333</v>
-      </c>
-      <c r="G2" t="s">
-        <v>334</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="M2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="P2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="Q2" t="s">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -38314,7 +38314,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1048576"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38422,7 +38422,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B5">
         <v>120006</v>
@@ -38560,7 +38560,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B11">
         <v>61360</v>
@@ -38768,7 +38768,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B5">
         <v>245600</v>
@@ -38906,7 +38906,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B11">
         <v>123901</v>
@@ -39114,7 +39114,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B5">
         <v>234960</v>
@@ -39252,7 +39252,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B11">
         <v>117924</v>

</xml_diff>